<commit_message>
Sử dụng Persistent Volume (pv) và Persistent Volume Claim (pvc) trong Kubernetes
</commit_message>
<xml_diff>
--- a/ReplicaSet-va-HPA-trong-Kubernetes/ReplicaSet-va-HPA-trong-Kubernetes.xlsx
+++ b/ReplicaSet-va-HPA-trong-Kubernetes/ReplicaSet-va-HPA-trong-Kubernetes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\kubernetes\ReplicaSet-va-HPA-trong-Kubernetes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8366E3-B580-43F0-BC15-56CA1F7424FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E5740F-54DE-47BC-9F8D-41DC372C31A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Thêm Kubernetes extension" sheetId="3" r:id="rId1"/>
@@ -3190,7 +3190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D59CA1D6-7459-40DE-A16B-58C085B16259}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3205,7 +3205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:B107"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
       <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
@@ -3640,7 +3640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D13BAE1-23A5-4F1A-9DD2-7A58BC9C4384}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>

</xml_diff>